<commit_message>
feedback form and other component updated
</commit_message>
<xml_diff>
--- a/FacultyFiles/ExcelList.xlsx
+++ b/FacultyFiles/ExcelList.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FacultyTbl" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Student" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -40,6 +40,45 @@
   </si>
   <si>
     <t>ruchivyas@gmail.com</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>sdjfhbhjb</t>
+  </si>
+  <si>
+    <t>FathersName</t>
+  </si>
+  <si>
+    <t>MothersName</t>
+  </si>
+  <si>
+    <t>FathersContactNo</t>
+  </si>
+  <si>
+    <t>MothersContactNo</t>
+  </si>
+  <si>
+    <t>ParentsLoginPassword</t>
+  </si>
+  <si>
+    <t>RollNo</t>
+  </si>
+  <si>
+    <t>16EGICS039</t>
+  </si>
+  <si>
+    <t>Himanshu Panchal</t>
+  </si>
+  <si>
+    <t>Mr. Rahul Panchal</t>
+  </si>
+  <si>
+    <t>Mrs. Jaya Panchal</t>
+  </si>
+  <si>
+    <t>panchalhimanshu@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -400,7 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -466,13 +505,103 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" customWidth="1"/>
+    <col min="6" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+    <col min="11" max="11" width="43.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>7410258963</v>
+      </c>
+      <c r="G2">
+        <v>9874563210</v>
+      </c>
+      <c r="H2">
+        <v>8520369147</v>
+      </c>
+      <c r="I2">
+        <v>111111</v>
+      </c>
+      <c r="J2">
+        <v>222222</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E3" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>